<commit_message>
Excel (xlsx) - Title Style 적용
</commit_message>
<xml_diff>
--- a/5_excel_db(xls)/VOC_20210817.xlsx
+++ b/5_excel_db(xls)/VOC_20210817.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +25,28 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <color rgb="00002060"/>
+      <sz val="16"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00e0e0e0"/>
+        <bgColor rgb="00ffff99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +54,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,17 +443,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>refID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>POI_ID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tag</t>
         </is>

</xml_diff>